<commit_message>
updated excel code-->feature file update
</commit_message>
<xml_diff>
--- a/PythonCode.xlsx
+++ b/PythonCode.xlsx
@@ -3,56 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="linkspythoncode" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="pythonCode" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="zuEuSZKJ0gh+ESz3IbOFptQIfN/N6MwG+Fy8rwGoBpg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="Goh0xeXyatuJXYxGKfk1r5C+Q/2syLKTmtQZdOx7Q2c="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>expectedmessage</t>
-  </si>
-  <si>
-    <t>Numpysdet84</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>Please check your password</t>
-  </si>
-  <si>
-    <t>sdet84batch</t>
-  </si>
-  <si>
-    <t>Please check your user id</t>
-  </si>
-  <si>
-    <t>You are logged in</t>
-  </si>
-  <si>
-    <t>Numpysdet86</t>
-  </si>
-  <si>
-    <t>sdet86batch</t>
-  </si>
-  <si>
-    <t>Invalid Username and Password</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+  <si>
+    <t>links</t>
   </si>
   <si>
     <t>pythonCode</t>
@@ -61,10 +28,28 @@
     <t>Result</t>
   </si>
   <si>
+    <t>arrays-in-python</t>
+  </si>
+  <si>
+    <t>print('hello')</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>arrays-using-list</t>
+  </si>
+  <si>
+    <t>basic-operations-in-lists</t>
+  </si>
+  <si>
+    <t>applications-of-array</t>
+  </si>
+  <si>
+    <t>NameError: name 'hello' is not defined on line 1</t>
+  </si>
+  <si>
     <t>print("hello");</t>
-  </si>
-  <si>
-    <t>hello</t>
   </si>
   <si>
     <t>def search(input_list, num):
@@ -124,6 +109,68 @@
   </si>
   <si>
     <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+  if(num in input_list):
+    print("Element Found
+  else:
+    print("Not Found")
+search([12, 23, 45, 67, 6, 90] , 12)</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 3</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+  result = 0
+  count = 0
+ for i in nums:
+    if i == 0:
+      count = 0 
+    else:
+      count+= 1
+      result = max(result, count) 
+  return result
+print(findMaxConsecutiveOnes([1,0,1,1,0,1]))</t>
+  </si>
+  <si>
+    <t>SyntaxError: unindent does not match any outer indentation level on line 4</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+  c=0
+  for i in nums:
+    j=str(i)
+    x=len(j)
+    if x%2==0:
+       c=c+1
+  print c
+ return c
+findNumbers([555,901,482,1771]</t>
+  </si>
+  <si>
+    <t>SyntaxError: unindent does not match any outer indentation level on line 9</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums)
+  squares_list = []
+  for i in range(0, len(nums)):
+    square = nums[i] * nums[i];
+    squares_list.append(square)
+  sorted_squares_list = sorted(squares_list)
+  print sorted_squares_list;
+  return sorted_squares_list;
+sortedSquares([-7,-3,2,3,11])</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>Enter Code before Run</t>
+  </si>
+  <si>
+    <t>No tests were collected</t>
   </si>
 </sst>
 </file>
@@ -143,47 +190,39 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -406,8 +445,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.43"/>
-    <col customWidth="1" min="2" max="2" width="11.71"/>
+    <col customWidth="1" min="1" max="1" width="21.29"/>
+    <col customWidth="1" min="2" max="2" width="11.57"/>
     <col customWidth="1" min="3" max="3" width="28.14"/>
     <col customWidth="1" min="4" max="6" width="8.71"/>
   </cols>
@@ -436,38 +475,86 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -1447,6 +1534,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -1472,91 +1560,133 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
+      <c r="A4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>22</v>
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
+      <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>